<commit_message>
added an approach stage and hard coded the crush velocity
</commit_message>
<xml_diff>
--- a/output/Test 181027/slow_to_stop_tests.xlsx
+++ b/output/Test 181027/slow_to_stop_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattmacdonald/Gitlab/crush-rig/output/Test 181027/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BCC573-A2F9-C84F-BCAF-CA5CC262F78D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2725527-DD88-E242-A297-800E9C8637D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1440" windowWidth="27240" windowHeight="16060" activeTab="1" xr2:uid="{B6D70832-2B77-594A-BAD2-BA1683C3B27E}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Timestamp (s)</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>bit of a slow down when changin speed</t>
+  </si>
+  <si>
+    <t>force - avg(5)</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -30066,13 +30078,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -30104,13 +30116,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>349250</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -41373,10 +41385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E86218F-AC75-EC44-AE3B-8517A7A0FFAC}">
-  <dimension ref="A1:I557"/>
+  <dimension ref="A1:M557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="104" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="104" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41387,9 +41399,11 @@
     <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -41409,7 +41423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4.8615999999999999E-2</v>
       </c>
@@ -41428,15 +41442,15 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <f>1*9.81</f>
         <v>9.81</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8.0588999999999994E-2</v>
       </c>
@@ -41455,15 +41469,15 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <f>1/AVERAGE(A10-A9,A9-A8,A8-A7,A7-A6,A6-A5,A5-A4,A4-A3,A3-A2)</f>
         <v>31.243287574935067</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.11262</v>
       </c>
@@ -41483,7 +41497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.14463899999999999</v>
       </c>
@@ -41503,7 +41517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.176645</v>
       </c>
@@ -41523,7 +41537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.20863100000000001</v>
       </c>
@@ -41543,7 +41557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.240651</v>
       </c>
@@ -41563,7 +41577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.27275300000000002</v>
       </c>
@@ -41583,7 +41597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.30467100000000003</v>
       </c>
@@ -41603,7 +41617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.33716099999999999</v>
       </c>
@@ -41623,7 +41637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.36877100000000002</v>
       </c>
@@ -41643,7 +41657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.40076299999999998</v>
       </c>
@@ -41663,7 +41677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.43274000000000001</v>
       </c>
@@ -41683,7 +41697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.46472400000000003</v>
       </c>
@@ -41703,7 +41717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.49677100000000002</v>
       </c>
@@ -42683,7 +42697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2.0658120000000002</v>
       </c>
@@ -42703,7 +42717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2.0976400000000002</v>
       </c>
@@ -42723,7 +42737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2.1294580000000001</v>
       </c>
@@ -42743,7 +42757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2.1618170000000001</v>
       </c>
@@ -42763,7 +42777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2.1937099999999998</v>
       </c>
@@ -42783,7 +42797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2.225749</v>
       </c>
@@ -42802,8 +42816,20 @@
       <c r="F70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2.2577729999999998</v>
       </c>
@@ -42822,8 +42848,24 @@
       <c r="F71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <f t="shared" ref="G71:G84" si="0">ABS(D71-AVERAGE(D67:D70))</f>
+        <v>2.0550000000000013E-2</v>
+      </c>
+      <c r="H71">
+        <f>_xlfn.STDEV.S(D67:D70)</f>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I71">
+        <f>MAX(D66:D70)</f>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J71">
+        <f>MIN(D65:D69)</f>
+        <v>-0.17419999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2.2899609999999999</v>
       </c>
@@ -42842,8 +42884,24 @@
       <c r="F72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <f t="shared" si="0"/>
+        <v>1.3700000000000018E-2</v>
+      </c>
+      <c r="H72">
+        <f t="shared" ref="H72:H98" si="1">_xlfn.STDEV.S(D68:D71)</f>
+        <v>1.5819397375795751E-2</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:I98" si="2">MAX(D67:D71)</f>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J72">
+        <f t="shared" ref="J72:J98" si="3">MIN(D66:D70)</f>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2.3219349999999999</v>
       </c>
@@ -42862,8 +42920,24 @@
       <c r="F73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <f t="shared" si="0"/>
+        <v>1.3700000000000018E-2</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>1.5819397375795751E-2</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="2"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2.3539850000000002</v>
       </c>
@@ -42882,8 +42956,24 @@
       <c r="F74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <f t="shared" si="0"/>
+        <v>1.3700000000000018E-2</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>1.5819397375795751E-2</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="2"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2.3858030000000001</v>
       </c>
@@ -42902,8 +42992,24 @@
       <c r="F75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <f t="shared" si="0"/>
+        <v>6.8500000000000227E-3</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="1"/>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="2"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2.4176419999999998</v>
       </c>
@@ -42922,8 +43028,24 @@
       <c r="F76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <f t="shared" si="0"/>
+        <v>2.7400000000000008E-2</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="2"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2.4498630000000001</v>
       </c>
@@ -42942,8 +43064,24 @@
       <c r="F77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <f t="shared" si="0"/>
+        <v>3.4249999999999975E-2</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="1"/>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2.481846</v>
       </c>
@@ -42962,8 +43100,24 @@
       <c r="F78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <f t="shared" si="0"/>
+        <v>2.7755575615628914E-17</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>2.2372006317419531E-2</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2.5138609999999999</v>
       </c>
@@ -42982,8 +43136,24 @@
       <c r="F79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <f t="shared" si="0"/>
+        <v>2.7755575615628914E-17</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="1"/>
+        <v>2.2372006317419431E-2</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2.5460600000000002</v>
       </c>
@@ -43002,8 +43172,24 @@
       <c r="F80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <f t="shared" si="0"/>
+        <v>2.7400000000000008E-2</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="1"/>
+        <v>2.2372006317419431E-2</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2.5780949999999998</v>
       </c>
@@ -43022,8 +43208,24 @@
       <c r="F81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <f t="shared" si="0"/>
+        <v>1.369999999999999E-2</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="1"/>
+        <v>1.5819397375795734E-2</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2.6100300000000001</v>
       </c>
@@ -43042,8 +43244,24 @@
       <c r="F82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <f t="shared" si="0"/>
+        <v>1.369999999999999E-2</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="1"/>
+        <v>1.5819397375795734E-2</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="3"/>
+        <v>-0.2016</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2.642334</v>
       </c>
@@ -43062,8 +43280,24 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <f t="shared" si="0"/>
+        <v>3.4250000000000003E-2</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="1"/>
+        <v>1.3699999999999992E-2</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="2"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="3"/>
+        <v>-0.17419999999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2.6742560000000002</v>
       </c>
@@ -43082,11 +43316,27 @@
       <c r="F84">
         <v>0</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84">
+        <f t="shared" si="0"/>
+        <v>6.849999999999995E-3</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="1"/>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="2"/>
+        <v>-0.11940000000000001</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="3"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="K84" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2.705991</v>
       </c>
@@ -43106,11 +43356,27 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <f t="shared" ref="G85:G88" si="0">D85-D84</f>
+        <f>ABS(D85-AVERAGE(D81:D84))</f>
+        <v>4.795000000000002E-2</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="1"/>
+        <v>1.3700000000000004E-2</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="2"/>
+        <v>-0.11940000000000001</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="3"/>
+        <v>-0.17419999999999999</v>
+      </c>
+      <c r="K85">
+        <f>D85-D84</f>
         <v>5.4800000000000015E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2.7379280000000001</v>
       </c>
@@ -43130,14 +43396,30 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G86:G98" si="4">ABS(D86-AVERAGE(D82:D85))</f>
+        <v>0.17125000000000001</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="1"/>
+        <v>2.6233502752523785E-2</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="3"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="K86">
+        <f>D86-D85</f>
         <v>0.13700000000000001</v>
       </c>
-      <c r="H86" t="s">
+      <c r="L86" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2.7701980000000002</v>
       </c>
@@ -43157,15 +43439,31 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
+        <v>0.26029999999999998</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>8.5190062018211193E-2</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="2"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="3"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="K87">
+        <f>D87-D86</f>
         <v>0.13700000000000001</v>
       </c>
-      <c r="H87">
-        <f t="shared" ref="H87:H96" si="1">1/(A87-A86)</f>
+      <c r="L87">
+        <f>1/(A87-A86)</f>
         <v>30.988534242330317</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2.802054</v>
       </c>
@@ -43185,15 +43483,31 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <f t="shared" si="0"/>
-        <v>0.24659999999999999</v>
+        <f t="shared" si="4"/>
+        <v>0.43154999999999999</v>
       </c>
       <c r="H88">
         <f t="shared" si="1"/>
+        <v>0.14734136101810202</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>0.182</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="3"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="K88">
+        <f>D88-D87</f>
+        <v>0.24659999999999999</v>
+      </c>
+      <c r="L88">
+        <f>1/(A88-A87)</f>
         <v>31.391260673028743</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2.834003</v>
       </c>
@@ -43213,15 +43527,31 @@
         <v>0</v>
       </c>
       <c r="G89">
+        <f t="shared" si="4"/>
+        <v>0.5343</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="1"/>
+        <v>0.22203582293554947</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="3"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="K89">
         <f>D89-D88</f>
         <v>0.24660000000000004</v>
       </c>
-      <c r="H89">
-        <f t="shared" si="1"/>
+      <c r="L89">
+        <f>1/(A89-A88)</f>
         <v>31.299884190428489</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2.8818229999999998</v>
       </c>
@@ -43241,18 +43571,34 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <f t="shared" ref="G90:G153" si="2">D90-D89</f>
-        <v>0.35620000000000007</v>
+        <f t="shared" si="4"/>
+        <v>0.6987000000000001</v>
       </c>
       <c r="H90">
         <f t="shared" si="1"/>
+        <v>0.27807962888352677</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="2"/>
+        <v>0.67520000000000002</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="3"/>
+        <v>-0.14680000000000001</v>
+      </c>
+      <c r="K90">
+        <f>D90-D89</f>
+        <v>0.35620000000000007</v>
+      </c>
+      <c r="L90">
+        <f>1/(A90-A89)</f>
         <v>20.911752404851637</v>
       </c>
-      <c r="I90" t="s">
+      <c r="M90" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2.9296899999999999</v>
       </c>
@@ -43272,15 +43618,31 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <f t="shared" si="2"/>
-        <v>0.38359999999999994</v>
+        <f t="shared" si="4"/>
+        <v>0.8357</v>
       </c>
       <c r="H91">
         <f t="shared" si="1"/>
+        <v>0.36246792961584895</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="2"/>
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="3"/>
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="K91">
+        <f>D91-D90</f>
+        <v>0.38359999999999994</v>
+      </c>
+      <c r="L91">
+        <f>1/(A91-A90)</f>
         <v>20.89121942047753</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2.9621219999999999</v>
       </c>
@@ -43300,15 +43662,31 @@
         <v>0</v>
       </c>
       <c r="G92">
+        <f t="shared" si="4"/>
+        <v>0.69184999999999985</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="1"/>
+        <v>0.42997052224542087</v>
+      </c>
+      <c r="I92">
         <f t="shared" si="2"/>
+        <v>1.415</v>
+      </c>
+      <c r="J92">
+        <f t="shared" si="3"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="K92">
+        <f>D92-D91</f>
         <v>0.16439999999999988</v>
       </c>
-      <c r="H92">
+      <c r="L92">
         <f>1/(A92-A91)</f>
         <v>30.833744449925984</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2.993919</v>
       </c>
@@ -43328,15 +43706,31 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <f t="shared" si="2"/>
-        <v>2.7400000000000091E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.4315500000000001</v>
       </c>
       <c r="H93">
         <f t="shared" si="1"/>
+        <v>0.40478805565382026</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="2"/>
+        <v>1.5793999999999999</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="3"/>
+        <v>0.182</v>
+      </c>
+      <c r="K93">
+        <f>D93-D92</f>
+        <v>2.7400000000000091E-2</v>
+      </c>
+      <c r="L93">
+        <f>1/(A93-A92)</f>
         <v>31.449507815202619</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>3.0262980000000002</v>
       </c>
@@ -43356,15 +43750,31 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <f t="shared" si="2"/>
-        <v>0.10959999999999992</v>
+        <f t="shared" si="4"/>
+        <v>0.30824999999999991</v>
       </c>
       <c r="H94">
         <f t="shared" si="1"/>
+        <v>0.26506343265968169</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="2"/>
+        <v>1.6068</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="3"/>
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="K94">
+        <f>D94-D93</f>
+        <v>0.10959999999999992</v>
+      </c>
+      <c r="L94">
+        <f>1/(A94-A93)</f>
         <v>30.884215077673652</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>3.0581459999999998</v>
       </c>
@@ -43384,15 +43794,31 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <f t="shared" si="2"/>
-        <v>2.7400000000000091E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.1644000000000001</v>
       </c>
       <c r="H95">
         <f t="shared" si="1"/>
+        <v>0.12456205949913744</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="2"/>
+        <v>1.7163999999999999</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="3"/>
+        <v>0.67520000000000002</v>
+      </c>
+      <c r="K95">
+        <f>D95-D94</f>
+        <v>2.7400000000000091E-2</v>
+      </c>
+      <c r="L95">
+        <f>1/(A95-A94)</f>
         <v>31.399145943230685</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>3.0908310000000001</v>
       </c>
@@ -43412,15 +43838,31 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <f t="shared" si="2"/>
-        <v>0.10959999999999992</v>
+        <f t="shared" si="4"/>
+        <v>0.19179999999999997</v>
       </c>
       <c r="H96">
         <f t="shared" si="1"/>
+        <v>8.0663415912461012E-2</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="2"/>
+        <v>1.7438</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="3"/>
+        <v>1.0314000000000001</v>
+      </c>
+      <c r="K96">
+        <f>D96-D95</f>
+        <v>0.10959999999999992</v>
+      </c>
+      <c r="L96">
+        <f>1/(A96-A95)</f>
         <v>30.595074193054639</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>3.1220460000000001</v>
       </c>
@@ -43440,11 +43882,27 @@
         <v>0</v>
       </c>
       <c r="G97">
+        <f t="shared" si="4"/>
+        <v>0.20550000000000002</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="1"/>
+        <v>0.10129356675853932</v>
+      </c>
+      <c r="I97">
         <f t="shared" si="2"/>
+        <v>1.8533999999999999</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="3"/>
+        <v>1.415</v>
+      </c>
+      <c r="K97">
+        <f>D97-D96</f>
         <v>8.2200000000000051E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>3.1541350000000001</v>
       </c>
@@ -43464,11 +43922,27 @@
         <v>0</v>
       </c>
       <c r="G98">
+        <f t="shared" si="4"/>
+        <v>0.17809999999999993</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="1"/>
+        <v>0.10129356675853934</v>
+      </c>
+      <c r="I98">
         <f t="shared" si="2"/>
+        <v>1.9356</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="3"/>
+        <v>1.5793999999999999</v>
+      </c>
+      <c r="K98">
+        <f>D98-D97</f>
         <v>5.479999999999996E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>3.1863169999999998</v>
       </c>
@@ -43487,12 +43961,12 @@
       <c r="F99">
         <v>0</v>
       </c>
-      <c r="G99">
-        <f t="shared" si="2"/>
+      <c r="K99">
+        <f>D99-D98</f>
         <v>8.2200000000000051E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>3.2182979999999999</v>
       </c>
@@ -43511,12 +43985,12 @@
       <c r="F100">
         <v>0</v>
       </c>
-      <c r="G100">
-        <f t="shared" si="2"/>
+      <c r="K100">
+        <f>D100-D99</f>
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>3.2501350000000002</v>
       </c>
@@ -43535,12 +44009,12 @@
       <c r="F101">
         <v>0</v>
       </c>
-      <c r="G101">
-        <f t="shared" si="2"/>
+      <c r="K101">
+        <f>D101-D100</f>
         <v>5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>3.28241</v>
       </c>
@@ -43559,12 +44033,12 @@
       <c r="F102">
         <v>0</v>
       </c>
-      <c r="G102">
-        <f t="shared" si="2"/>
+      <c r="K102">
+        <f>D102-D101</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>3.314384</v>
       </c>
@@ -43583,12 +44057,12 @@
       <c r="F103">
         <v>0</v>
       </c>
-      <c r="G103">
-        <f t="shared" si="2"/>
+      <c r="K103">
+        <f>D103-D102</f>
         <v>8.2199999999999829E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>3.3464589999999999</v>
       </c>
@@ -43607,12 +44081,12 @@
       <c r="F104">
         <v>0</v>
       </c>
-      <c r="G104">
-        <f t="shared" si="2"/>
+      <c r="K104">
+        <f>D104-D103</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>3.3783720000000002</v>
       </c>
@@ -43631,12 +44105,12 @@
       <c r="F105">
         <v>0</v>
       </c>
-      <c r="G105">
-        <f t="shared" si="2"/>
+      <c r="K105">
+        <f>D105-D104</f>
         <v>8.2200000000000273E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>3.4105620000000001</v>
       </c>
@@ -43655,12 +44129,12 @@
       <c r="F106">
         <v>0</v>
       </c>
-      <c r="G106">
-        <f t="shared" si="2"/>
+      <c r="K106">
+        <f>D106-D105</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>3.4425650000000001</v>
       </c>
@@ -43679,12 +44153,12 @@
       <c r="F107">
         <v>0</v>
       </c>
-      <c r="G107">
-        <f t="shared" si="2"/>
+      <c r="K107">
+        <f>D107-D106</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>3.474599</v>
       </c>
@@ -43703,12 +44177,12 @@
       <c r="F108">
         <v>0</v>
       </c>
-      <c r="G108">
-        <f t="shared" si="2"/>
+      <c r="K108">
+        <f>D108-D107</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>3.5063800000000001</v>
       </c>
@@ -43727,12 +44201,12 @@
       <c r="F109">
         <v>0</v>
       </c>
-      <c r="G109">
-        <f t="shared" si="2"/>
+      <c r="K109">
+        <f>D109-D108</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>3.5383710000000002</v>
       </c>
@@ -43751,12 +44225,12 @@
       <c r="F110">
         <v>0</v>
       </c>
-      <c r="G110">
-        <f t="shared" si="2"/>
+      <c r="K110">
+        <f>D110-D109</f>
         <v>8.2200000000000273E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>3.5704120000000001</v>
       </c>
@@ -43775,12 +44249,12 @@
       <c r="F111">
         <v>0</v>
       </c>
-      <c r="G111">
-        <f t="shared" si="2"/>
+      <c r="K111">
+        <f>D111-D110</f>
         <v>8.2199999999999829E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>3.602554</v>
       </c>
@@ -43799,12 +44273,12 @@
       <c r="F112">
         <v>0</v>
       </c>
-      <c r="G112">
-        <f t="shared" si="2"/>
+      <c r="K112">
+        <f>D112-D111</f>
         <v>0.19180000000000019</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>3.634223</v>
       </c>
@@ -43823,12 +44297,12 @@
       <c r="F113">
         <v>0</v>
       </c>
-      <c r="G113">
-        <f t="shared" si="2"/>
+      <c r="K113">
+        <f>D113-D112</f>
         <v>8.2199999999999829E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>3.6666439999999998</v>
       </c>
@@ -43847,12 +44321,12 @@
       <c r="F114">
         <v>0</v>
       </c>
-      <c r="G114">
-        <f t="shared" si="2"/>
+      <c r="K114">
+        <f>D114-D113</f>
         <v>0.10959999999999992</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>3.698642</v>
       </c>
@@ -43871,12 +44345,12 @@
       <c r="F115">
         <v>0</v>
       </c>
-      <c r="G115">
-        <f t="shared" si="2"/>
+      <c r="K115">
+        <f>D115-D114</f>
         <v>0.1644000000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>3.7305030000000001</v>
       </c>
@@ -43895,12 +44369,12 @@
       <c r="F116">
         <v>0</v>
       </c>
-      <c r="G116">
-        <f t="shared" si="2"/>
+      <c r="K116">
+        <f>D116-D115</f>
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>3.7625799999999998</v>
       </c>
@@ -43919,12 +44393,12 @@
       <c r="F117">
         <v>0</v>
       </c>
-      <c r="G117">
-        <f t="shared" si="2"/>
+      <c r="K117">
+        <f>D117-D116</f>
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>3.7946650000000002</v>
       </c>
@@ -43943,12 +44417,12 @@
       <c r="F118">
         <v>0</v>
       </c>
-      <c r="G118">
-        <f t="shared" si="2"/>
+      <c r="K118">
+        <f>D118-D117</f>
         <v>0.16439999999999966</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>3.8266149999999999</v>
       </c>
@@ -43967,12 +44441,12 @@
       <c r="F119">
         <v>0</v>
       </c>
-      <c r="G119">
-        <f t="shared" si="2"/>
+      <c r="K119">
+        <f>D119-D118</f>
         <v>0.16440000000000055</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>3.8586200000000002</v>
       </c>
@@ -43991,12 +44465,12 @@
       <c r="F120">
         <v>0</v>
       </c>
-      <c r="G120">
-        <f t="shared" si="2"/>
+      <c r="K120">
+        <f>D120-D119</f>
         <v>0.16439999999999966</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>3.8906260000000001</v>
       </c>
@@ -44015,15 +44489,15 @@
       <c r="F121">
         <v>0</v>
       </c>
-      <c r="G121">
-        <f t="shared" si="2"/>
+      <c r="K121">
+        <f>D121-D120</f>
         <v>0.16440000000000055</v>
       </c>
-      <c r="H121" t="s">
+      <c r="L121" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>3.9226930000000002</v>
       </c>
@@ -44042,16 +44516,16 @@
       <c r="F122">
         <v>0</v>
       </c>
-      <c r="G122">
-        <f t="shared" si="2"/>
+      <c r="K122">
+        <f>D122-D121</f>
         <v>0.21919999999999984</v>
       </c>
-      <c r="H122">
-        <f t="shared" ref="H122:H127" si="3">1/(A122-A121)</f>
+      <c r="L122">
+        <f>1/(A122-A121)</f>
         <v>31.184707019677486</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>3.9546540000000001</v>
       </c>
@@ -44070,16 +44544,16 @@
       <c r="F123">
         <v>0</v>
       </c>
-      <c r="G123">
-        <f t="shared" si="2"/>
+      <c r="K123">
+        <f>D123-D122</f>
         <v>0.16439999999999966</v>
       </c>
-      <c r="H123">
-        <f t="shared" si="3"/>
+      <c r="L123">
+        <f>1/(A123-A122)</f>
         <v>31.288132411376456</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>4.0024490000000004</v>
       </c>
@@ -44098,16 +44572,16 @@
       <c r="F124">
         <v>0</v>
       </c>
-      <c r="G124">
-        <f t="shared" si="2"/>
+      <c r="K124">
+        <f>D124-D123</f>
         <v>0.27400000000000002</v>
       </c>
-      <c r="H124">
-        <f t="shared" si="3"/>
+      <c r="L124">
+        <f>1/(A124-A123)</f>
         <v>20.92269065801851</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>4.0346979999999997</v>
       </c>
@@ -44126,16 +44600,16 @@
       <c r="F125">
         <v>0</v>
       </c>
-      <c r="G125">
-        <f t="shared" si="2"/>
+      <c r="K125">
+        <f>D125-D124</f>
         <v>0.19179999999999975</v>
       </c>
-      <c r="H125">
-        <f t="shared" si="3"/>
+      <c r="L125">
+        <f>1/(A125-A124)</f>
         <v>31.008713448479689</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>4.0667859999999996</v>
       </c>
@@ -44154,16 +44628,16 @@
       <c r="F126">
         <v>0</v>
       </c>
-      <c r="G126">
-        <f t="shared" si="2"/>
+      <c r="K126">
+        <f>D126-D125</f>
         <v>0.13700000000000045</v>
       </c>
-      <c r="H126">
+      <c r="L126">
         <f>1/(A126-A125)</f>
         <v>31.16429818000509</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>4.0987859999999996</v>
       </c>
@@ -44182,16 +44656,16 @@
       <c r="F127">
         <v>0</v>
       </c>
-      <c r="G127">
-        <f t="shared" si="2"/>
+      <c r="K127">
+        <f>D127-D126</f>
         <v>0.21919999999999984</v>
       </c>
-      <c r="H127">
-        <f t="shared" si="3"/>
+      <c r="L127">
+        <f>1/(A127-A126)</f>
         <v>31.249999999999972</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>4.1309639999999996</v>
       </c>
@@ -44210,12 +44684,12 @@
       <c r="F128">
         <v>0</v>
       </c>
-      <c r="G128">
-        <f t="shared" si="2"/>
+      <c r="K128">
+        <f>D128-D127</f>
         <v>0.13700000000000045</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>4.1630919999999998</v>
       </c>
@@ -44234,12 +44708,12 @@
       <c r="F129">
         <v>0</v>
       </c>
-      <c r="G129">
-        <f t="shared" si="2"/>
+      <c r="K129">
+        <f>D129-D128</f>
         <v>0.24659999999999993</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>4.1948189999999999</v>
       </c>
@@ -44258,12 +44732,12 @@
       <c r="F130">
         <v>0</v>
       </c>
-      <c r="G130">
-        <f t="shared" si="2"/>
+      <c r="K130">
+        <f>D130-D129</f>
         <v>0.16439999999999966</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>4.2271890000000001</v>
       </c>
@@ -44282,12 +44756,12 @@
       <c r="F131">
         <v>0</v>
       </c>
-      <c r="G131">
-        <f t="shared" si="2"/>
+      <c r="K131">
+        <f>D131-D130</f>
         <v>0.24659999999999993</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>4.2586250000000003</v>
       </c>
@@ -44306,12 +44780,12 @@
       <c r="F132">
         <v>0</v>
       </c>
-      <c r="G132">
-        <f t="shared" si="2"/>
+      <c r="K132">
+        <f>D132-D131</f>
         <v>0.21919999999999984</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>4.2905199999999999</v>
       </c>
@@ -44330,12 +44804,12 @@
       <c r="F133">
         <v>0</v>
       </c>
-      <c r="G133">
-        <f t="shared" si="2"/>
+      <c r="K133">
+        <f>D133-D132</f>
         <v>0.21919999999999984</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>4.3228489999999997</v>
       </c>
@@ -44354,12 +44828,12 @@
       <c r="F134">
         <v>0</v>
       </c>
-      <c r="G134">
-        <f t="shared" si="2"/>
+      <c r="K134">
+        <f>D134-D133</f>
         <v>0.21920000000000073</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>4.3548229999999997</v>
       </c>
@@ -44378,12 +44852,12 @@
       <c r="F135">
         <v>0</v>
       </c>
-      <c r="G135">
-        <f t="shared" si="2"/>
+      <c r="K135">
+        <f>D135-D134</f>
         <v>0.27400000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>4.3870120000000004</v>
       </c>
@@ -44402,12 +44876,12 @@
       <c r="F136">
         <v>0</v>
       </c>
-      <c r="G136">
-        <f t="shared" si="2"/>
+      <c r="K136">
+        <f>D136-D135</f>
         <v>0.30139999999999922</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>4.4189090000000002</v>
       </c>
@@ -44426,12 +44900,12 @@
       <c r="F137">
         <v>0</v>
       </c>
-      <c r="G137">
-        <f t="shared" si="2"/>
+      <c r="K137">
+        <f>D137-D136</f>
         <v>0.27400000000000091</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>4.4508939999999999</v>
       </c>
@@ -44450,12 +44924,12 @@
       <c r="F138">
         <v>0</v>
       </c>
-      <c r="G138">
-        <f t="shared" si="2"/>
+      <c r="K138">
+        <f>D138-D137</f>
         <v>0.32879999999999932</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>4.4829929999999996</v>
       </c>
@@ -44474,12 +44948,12 @@
       <c r="F139">
         <v>0</v>
       </c>
-      <c r="G139">
-        <f t="shared" si="2"/>
+      <c r="K139">
+        <f>D139-D138</f>
         <v>0.301400000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>4.5151349999999999</v>
       </c>
@@ -44498,12 +44972,12 @@
       <c r="F140">
         <v>0</v>
       </c>
-      <c r="G140">
-        <f t="shared" si="2"/>
+      <c r="K140">
+        <f>D140-D139</f>
         <v>0.3835999999999995</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>4.5468760000000001</v>
       </c>
@@ -44522,12 +44996,12 @@
       <c r="F141">
         <v>0</v>
       </c>
-      <c r="G141">
-        <f t="shared" si="2"/>
+      <c r="K141">
+        <f>D141-D140</f>
         <v>0.32879999999999932</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>4.594544</v>
       </c>
@@ -44546,19 +45020,19 @@
       <c r="F142">
         <v>1</v>
       </c>
-      <c r="G142">
-        <f t="shared" si="2"/>
+      <c r="K142">
+        <f>D142-D141</f>
         <v>0.38360000000000127</v>
       </c>
-      <c r="H142">
-        <f>100*(MAX(D140:D145)-H2)/H2</f>
+      <c r="L142">
+        <f>100*(MAX(D140:D145)-K2)/K2</f>
         <v>2.6850152905198672</v>
       </c>
-      <c r="I142" t="s">
+      <c r="M142" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>4.6269200000000001</v>
       </c>
@@ -44577,12 +45051,12 @@
       <c r="F143">
         <v>1</v>
       </c>
-      <c r="G143">
-        <f t="shared" si="2"/>
+      <c r="K143">
+        <f>D143-D142</f>
         <v>0.10959999999999859</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>4.6585760000000001</v>
       </c>
@@ -44601,12 +45075,12 @@
       <c r="F144">
         <v>1</v>
       </c>
-      <c r="G144">
-        <f t="shared" si="2"/>
+      <c r="K144">
+        <f>D144-D143</f>
         <v>-0.10959999999999859</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>4.6910910000000001</v>
       </c>
@@ -44625,12 +45099,12 @@
       <c r="F145">
         <v>1</v>
       </c>
-      <c r="G145">
-        <f t="shared" si="2"/>
+      <c r="K145">
+        <f>D145-D144</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>4.7229099999999997</v>
       </c>
@@ -44649,12 +45123,12 @@
       <c r="F146">
         <v>1</v>
       </c>
-      <c r="G146">
-        <f t="shared" si="2"/>
+      <c r="K146">
+        <f>D146-D145</f>
         <v>-0.10960000000000036</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>4.7547389999999998</v>
       </c>
@@ -44673,12 +45147,12 @@
       <c r="F147">
         <v>1</v>
       </c>
-      <c r="G147">
-        <f t="shared" si="2"/>
+      <c r="K147">
+        <f>D147-D146</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>4.787045</v>
       </c>
@@ -44697,12 +45171,12 @@
       <c r="F148">
         <v>1</v>
       </c>
-      <c r="G148">
-        <f t="shared" si="2"/>
+      <c r="K148">
+        <f>D148-D147</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>4.8190710000000001</v>
       </c>
@@ -44721,12 +45195,12 @@
       <c r="F149">
         <v>1</v>
       </c>
-      <c r="G149">
-        <f t="shared" si="2"/>
+      <c r="K149">
+        <f>D149-D148</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>4.8509370000000001</v>
       </c>
@@ -44745,12 +45219,12 @@
       <c r="F150">
         <v>1</v>
       </c>
-      <c r="G150">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K150">
+        <f>D150-D149</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>4.88293</v>
       </c>
@@ -44769,12 +45243,12 @@
       <c r="F151">
         <v>1</v>
       </c>
-      <c r="G151">
-        <f t="shared" si="2"/>
+      <c r="K151">
+        <f>D151-D150</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>4.9151239999999996</v>
       </c>
@@ -44793,12 +45267,12 @@
       <c r="F152">
         <v>1</v>
       </c>
-      <c r="G152">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K152">
+        <f>D152-D151</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>4.9468500000000004</v>
       </c>
@@ -44817,12 +45291,12 @@
       <c r="F153">
         <v>1</v>
       </c>
-      <c r="G153">
-        <f t="shared" si="2"/>
+      <c r="K153">
+        <f>D153-D152</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>4.9788870000000003</v>
       </c>
@@ -44841,12 +45315,12 @@
       <c r="F154">
         <v>1</v>
       </c>
-      <c r="G154">
-        <f t="shared" ref="G154:G180" si="4">D154-D153</f>
+      <c r="K154">
+        <f>D154-D153</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>5.0109690000000002</v>
       </c>
@@ -44865,12 +45339,12 @@
       <c r="F155">
         <v>1</v>
       </c>
-      <c r="G155">
-        <f t="shared" si="4"/>
+      <c r="K155">
+        <f>D155-D154</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>5.0430260000000002</v>
       </c>
@@ -44889,12 +45363,12 @@
       <c r="F156">
         <v>1</v>
       </c>
-      <c r="G156">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K156">
+        <f>D156-D155</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>5.075151</v>
       </c>
@@ -44913,12 +45387,12 @@
       <c r="F157">
         <v>1</v>
       </c>
-      <c r="G157">
-        <f t="shared" si="4"/>
+      <c r="K157">
+        <f>D157-D156</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>5.1071530000000003</v>
       </c>
@@ -44937,12 +45411,12 @@
       <c r="F158">
         <v>1</v>
       </c>
-      <c r="G158">
-        <f t="shared" si="4"/>
+      <c r="K158">
+        <f>D158-D157</f>
         <v>5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>5.1391470000000004</v>
       </c>
@@ -44961,12 +45435,12 @@
       <c r="F159">
         <v>1</v>
       </c>
-      <c r="G159">
-        <f t="shared" si="4"/>
+      <c r="K159">
+        <f>D159-D158</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>5.1713100000000001</v>
       </c>
@@ -44985,12 +45459,12 @@
       <c r="F160">
         <v>1</v>
       </c>
-      <c r="G160">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K160">
+        <f>D160-D159</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>5.2032740000000004</v>
       </c>
@@ -45009,12 +45483,12 @@
       <c r="F161">
         <v>1</v>
       </c>
-      <c r="G161">
-        <f t="shared" si="4"/>
+      <c r="K161">
+        <f>D161-D160</f>
         <v>5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>5.234934</v>
       </c>
@@ -45033,12 +45507,12 @@
       <c r="F162">
         <v>1</v>
       </c>
-      <c r="G162">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K162">
+        <f>D162-D161</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>5.267315</v>
       </c>
@@ -45057,12 +45531,12 @@
       <c r="F163">
         <v>1</v>
       </c>
-      <c r="G163">
-        <f t="shared" si="4"/>
+      <c r="K163">
+        <f>D163-D162</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>5.2991780000000004</v>
       </c>
@@ -45081,12 +45555,12 @@
       <c r="F164">
         <v>1</v>
       </c>
-      <c r="G164">
-        <f t="shared" si="4"/>
+      <c r="K164">
+        <f>D164-D163</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>5.3313540000000001</v>
       </c>
@@ -45105,12 +45579,12 @@
       <c r="F165">
         <v>1</v>
       </c>
-      <c r="G165">
-        <f t="shared" si="4"/>
+      <c r="K165">
+        <f>D165-D164</f>
         <v>5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>5.3633870000000003</v>
       </c>
@@ -45129,12 +45603,12 @@
       <c r="F166">
         <v>1</v>
       </c>
-      <c r="G166">
-        <f t="shared" si="4"/>
+      <c r="K166">
+        <f>D166-D165</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>5.3952910000000003</v>
       </c>
@@ -45153,12 +45627,12 @@
       <c r="F167">
         <v>1</v>
       </c>
-      <c r="G167">
-        <f t="shared" si="4"/>
+      <c r="K167">
+        <f>D167-D166</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>5.4272939999999998</v>
       </c>
@@ -45177,12 +45651,12 @@
       <c r="F168">
         <v>1</v>
       </c>
-      <c r="G168">
-        <f t="shared" si="4"/>
+      <c r="K168">
+        <f>D168-D167</f>
         <v>-8.2200000000000273E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>5.4590759999999996</v>
       </c>
@@ -45201,12 +45675,12 @@
       <c r="F169">
         <v>1</v>
       </c>
-      <c r="G169">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K169">
+        <f>D169-D168</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>5.4915060000000002</v>
       </c>
@@ -45225,12 +45699,12 @@
       <c r="F170">
         <v>1</v>
       </c>
-      <c r="G170">
-        <f t="shared" si="4"/>
+      <c r="K170">
+        <f>D170-D169</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>5.5231960000000004</v>
       </c>
@@ -45249,12 +45723,12 @@
       <c r="F171">
         <v>1</v>
       </c>
-      <c r="G171">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K171">
+        <f>D171-D170</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>5.5553419999999996</v>
       </c>
@@ -45273,12 +45747,12 @@
       <c r="F172">
         <v>1</v>
       </c>
-      <c r="G172">
-        <f t="shared" si="4"/>
+      <c r="K172">
+        <f>D172-D171</f>
         <v>5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>5.5873619999999997</v>
       </c>
@@ -45297,12 +45771,12 @@
       <c r="F173">
         <v>1</v>
       </c>
-      <c r="G173">
-        <f t="shared" si="4"/>
+      <c r="K173">
+        <f>D173-D172</f>
         <v>-2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>5.6193939999999998</v>
       </c>
@@ -45321,12 +45795,12 @@
       <c r="F174">
         <v>1</v>
       </c>
-      <c r="G174">
-        <f t="shared" si="4"/>
+      <c r="K174">
+        <f>D174-D173</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>5.6514150000000001</v>
       </c>
@@ -45345,12 +45819,12 @@
       <c r="F175">
         <v>1</v>
       </c>
-      <c r="G175">
-        <f t="shared" si="4"/>
+      <c r="K175">
+        <f>D175-D174</f>
         <v>8.2200000000000273E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>5.6836029999999997</v>
       </c>
@@ -45369,12 +45843,12 @@
       <c r="F176">
         <v>1</v>
       </c>
-      <c r="G176">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K176">
+        <f>D176-D175</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>5.71549</v>
       </c>
@@ -45393,12 +45867,12 @@
       <c r="F177">
         <v>1</v>
       </c>
-      <c r="G177">
-        <f t="shared" si="4"/>
+      <c r="K177">
+        <f>D177-D176</f>
         <v>-8.2200000000000273E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>5.7475149999999999</v>
       </c>
@@ -45417,12 +45891,12 @@
       <c r="F178">
         <v>1</v>
       </c>
-      <c r="G178">
-        <f t="shared" si="4"/>
+      <c r="K178">
+        <f>D178-D177</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>5.7795949999999996</v>
       </c>
@@ -45441,12 +45915,12 @@
       <c r="F179">
         <v>1</v>
       </c>
-      <c r="G179">
-        <f t="shared" si="4"/>
+      <c r="K179">
+        <f>D179-D178</f>
         <v>-5.4800000000000182E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>5.8116979999999998</v>
       </c>
@@ -45465,12 +45939,12 @@
       <c r="F180">
         <v>1</v>
       </c>
-      <c r="G180">
-        <f t="shared" si="4"/>
+      <c r="K180">
+        <f>D180-D179</f>
         <v>2.7400000000000091E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>5.8434299999999997</v>
       </c>
@@ -45490,7 +45964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>5.8752570000000004</v>
       </c>
@@ -45510,7 +45984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>5.9075509999999998</v>
       </c>
@@ -45530,7 +46004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>5.9397609999999998</v>
       </c>
@@ -45550,7 +46024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>5.971565</v>
       </c>
@@ -45570,7 +46044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>6.0035869999999996</v>
       </c>
@@ -45590,7 +46064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>6.03538</v>
       </c>
@@ -45610,7 +46084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>6.0677529999999997</v>
       </c>
@@ -45630,7 +46104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>6.0997079999999997</v>
       </c>
@@ -45650,7 +46124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>6.1319480000000004</v>
       </c>
@@ -45670,7 +46144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>6.1635590000000002</v>
       </c>
@@ -45690,7 +46164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>6.1956889999999998</v>
       </c>

</xml_diff>